<commit_message>
#761 Create functional test for 'pull images' rule
</commit_message>
<xml_diff>
--- a/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-07-08/5_families.xlsx
+++ b/pim/src/PcmtCustomDatasetBundle/Resources/fixtures/pcmt_global/import_files/2020-07-08/5_families.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t xml:space="preserve">BASE_UOM,PRODUCT_DESCRIPTION,sku,UN_SUPPLY_MATERIAL_CODE,WHO_COVID19_ITEM_CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE_FAMILY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGE FAMILY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL_ATTRIBUTE,IMAGE_ATTRIBUTE,sku</t>
   </si>
 </sst>
 </file>
@@ -265,16 +274,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.44814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.462962962963"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.44814814814815"/>
   </cols>
   <sheetData>
@@ -489,6 +498,26 @@
       </c>
       <c r="I9" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>